<commit_message>
updated lab list spreadsheet
Now shows lab numbers for Fall 2015
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
@@ -24,7 +24,7 @@
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P18" authorId="0" shapeId="0">
+    <comment ref="Q18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N21" authorId="0" shapeId="0">
+    <comment ref="O21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>title</t>
   </si>
@@ -456,6 +456,10 @@
   <si>
     <t>Spr '16
 Henry</t>
+  </si>
+  <si>
+    <t>number,
+fall 2015</t>
   </si>
 </sst>
 </file>
@@ -1600,12 +1604,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="864" activePane="bottomLeft"/>
-      <selection activeCell="F1" activeCellId="9" sqref="F1:F1048576 F8 F7 F6 F5 F4 F3 F2 F1 F1"/>
-      <selection pane="bottomLeft" activeCell="R12" sqref="R12"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,17 +1617,17 @@
     <col min="1" max="1" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.5546875" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="44"/>
-    <col min="7" max="7" width="8.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.88671875" style="2"/>
-    <col min="11" max="11" width="8.88671875" style="35"/>
-    <col min="13" max="13" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" customWidth="1"/>
+    <col min="4" max="5" width="8.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="44"/>
+    <col min="8" max="8" width="8.21875" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="2"/>
+    <col min="12" max="12" width="8.88671875" style="35"/>
+    <col min="14" max="14" width="10.77734375" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
@@ -1636,42 +1640,45 @@
       <c r="D1" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>87</v>
       </c>
@@ -1684,13 +1691,10 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="F2" s="44">
-        <v>1</v>
-      </c>
       <c r="G2" s="44">
         <v>1</v>
       </c>
-      <c r="H2" s="45">
+      <c r="H2" s="44">
         <v>1</v>
       </c>
       <c r="I2" s="45">
@@ -1699,30 +1703,30 @@
       <c r="J2" s="45">
         <v>1</v>
       </c>
-      <c r="K2" s="35">
-        <f>SUM(G2:J2)</f>
+      <c r="K2" s="45">
+        <v>1</v>
+      </c>
+      <c r="L2" s="35">
+        <f>SUM(H2:K2)</f>
         <v>4</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="5"/>
+      <c r="N2" s="23"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>84</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="F3" s="44">
-        <v>1</v>
-      </c>
       <c r="G3" s="44">
         <v>1</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="44">
         <v>1</v>
       </c>
       <c r="I3" s="45">
@@ -1731,27 +1735,30 @@
       <c r="J3" s="45">
         <v>1</v>
       </c>
-      <c r="K3" s="35">
-        <f t="shared" ref="K3:K66" si="0">SUM(G3:J3)</f>
+      <c r="K3" s="45">
+        <v>1</v>
+      </c>
+      <c r="L3" s="35">
+        <f t="shared" ref="L3:L66" si="0">SUM(H3:K3)</f>
         <v>4</v>
       </c>
-      <c r="M3" s="23">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <f>SUMIF(K$2:K$81,"&gt;=" &amp; M3,C$2:C$81)</f>
+      <c r="N3" s="23">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <f>SUMIF(L$2:L$81,"&gt;=" &amp; N3,C$2:C$81)</f>
         <v>294</v>
       </c>
-      <c r="O3" s="6">
-        <f>SUMIF(K$2:K$81,"&gt;=" &amp; M3,D$2:D$81)</f>
+      <c r="P3" s="6">
+        <f>SUMIF(L$2:L$81,"&gt;=" &amp; N3,D$2:D$81)</f>
         <v>6</v>
       </c>
-      <c r="P3" s="9">
-        <f>($P$16 + $P$14*N3+($P$15)*O3)*(1+P$17+P$18)</f>
+      <c r="Q3" s="9">
+        <f>($Q$16 + $Q$14*O3+($Q$15)*P3)*(1+Q$17+Q$18)</f>
         <v>25.350000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>80</v>
       </c>
@@ -1762,491 +1769,527 @@
         <v>4</v>
       </c>
       <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="46">
-        <v>1</v>
-      </c>
-      <c r="G4" s="46"/>
-      <c r="H4" s="10"/>
+      <c r="E4" s="32">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="46">
+        <v>1</v>
+      </c>
+      <c r="H4" s="46"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="23">
+      <c r="K4" s="10"/>
+      <c r="L4" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="23">
         <v>0.5</v>
       </c>
-      <c r="N4" s="6">
-        <f t="shared" ref="N4:N11" si="1">SUMIF(K$2:K$81,"&gt;=" &amp; M4,C$2:C$81)</f>
+      <c r="O4" s="6">
+        <f t="shared" ref="O4:O11" si="1">SUMIF(L$2:L$81,"&gt;=" &amp; N4,C$2:C$81)</f>
         <v>4</v>
       </c>
-      <c r="O4" s="6">
-        <f t="shared" ref="O4:O11" si="2">SUMIF(K$2:K$81,"&gt;=" &amp; M4,D$2:D$81)</f>
-        <v>1</v>
-      </c>
-      <c r="P4" s="9">
-        <f t="shared" ref="P4:P11" si="3">($P$16 + $P$14*N4+($P$15)*O4)*(1+P$17+P$18)</f>
+      <c r="P4" s="6">
+        <f t="shared" ref="P4:P11" si="2">SUMIF(L$2:L$81,"&gt;=" &amp; N4,D$2:D$81)</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" ref="Q4:Q11" si="3">($Q$16 + $Q$14*O4+($Q$15)*P4)*(1+Q$17+Q$18)</f>
         <v>4.55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="K5" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="23">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="23">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="K6" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
+      <c r="L6" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
         <v>1.5</v>
       </c>
-      <c r="N6" s="19">
+      <c r="O6" s="19">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O6" s="19">
+      <c r="P6" s="19">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P6" s="20">
+      <c r="Q6" s="20">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="K7" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="23">
+      <c r="L7" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="23">
         <v>2</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P7" s="9">
+      <c r="Q7" s="9">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>94</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="K8" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="23">
+      <c r="L8" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="23">
         <v>2.5</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="F9" s="44">
-        <v>1</v>
-      </c>
-      <c r="K9" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="23">
+      <c r="E9">
         <v>3</v>
       </c>
-      <c r="N9" s="6">
+      <c r="G9" s="44">
+        <v>1</v>
+      </c>
+      <c r="L9" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="23">
+        <v>3</v>
+      </c>
+      <c r="O9" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="F10" s="44">
-        <v>1</v>
-      </c>
-      <c r="K10" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="23">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="44">
+        <v>1</v>
+      </c>
+      <c r="L10" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="23">
         <v>3.5</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O10" s="6">
+      <c r="P10" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="F11" s="44">
-        <v>1</v>
-      </c>
-      <c r="K11" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="25">
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="44">
+        <v>1</v>
+      </c>
+      <c r="L11" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="25">
         <v>4</v>
       </c>
-      <c r="N11" s="11">
+      <c r="O11" s="11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="O11" s="11">
+      <c r="P11" s="11">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P11" s="12">
+      <c r="Q11" s="12">
         <f t="shared" si="3"/>
         <v>4.55</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="K12" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
-      <c r="F13" s="44">
-        <v>1</v>
-      </c>
-      <c r="K13" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="1" t="s">
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="44">
+        <v>1</v>
+      </c>
+      <c r="L13" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="F14" s="44">
-        <v>1</v>
-      </c>
-      <c r="K14" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="14" t="s">
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="G14" s="44">
+        <v>1</v>
+      </c>
+      <c r="L14" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="41"/>
-      <c r="P14" s="13">
+      <c r="P14" s="41"/>
+      <c r="Q14" s="13">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15">
         <v>6</v>
       </c>
-      <c r="K15" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="15" t="s">
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="L15" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="9">
+      <c r="P15" s="5"/>
+      <c r="Q15" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>23</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="K16" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="15" t="s">
+      <c r="L16" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="9">
+      <c r="P16" s="5"/>
+      <c r="Q16" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>24</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="F17" s="44">
-        <v>1</v>
-      </c>
-      <c r="K17" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="15" t="s">
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="G17" s="44">
+        <v>1</v>
+      </c>
+      <c r="L17" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="43">
+      <c r="P17" s="5"/>
+      <c r="Q17" s="43">
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="F18" s="44">
-        <v>1</v>
-      </c>
-      <c r="K18" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="16" t="s">
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="44">
+        <v>1</v>
+      </c>
+      <c r="L18" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="O18" s="42"/>
-      <c r="P18" s="21">
+      <c r="P18" s="42"/>
+      <c r="Q18" s="21">
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>26</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="K19" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L19" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="K20" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="37" t="s">
+      <c r="L20" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="38"/>
-    </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="38"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="K21" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="39">
+      <c r="L21" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="39">
         <v>1.5</v>
       </c>
-      <c r="O21" s="40"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P21" s="40"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>29</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="K22" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L22" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>30</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="K23" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L23" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="F24" s="44">
-        <v>1</v>
-      </c>
-      <c r="K24" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>11</v>
+      </c>
+      <c r="G24" s="44">
+        <v>1</v>
+      </c>
+      <c r="L24" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>32</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="44">
-        <v>1</v>
-      </c>
-      <c r="K25" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G25" s="44">
+        <v>1</v>
+      </c>
+      <c r="L25" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="C26">
         <v>6</v>
       </c>
-      <c r="F26" s="44">
-        <v>1</v>
-      </c>
-      <c r="K26" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>12</v>
+      </c>
+      <c r="G26" s="44">
+        <v>1</v>
+      </c>
+      <c r="L26" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>79</v>
       </c>
@@ -2257,158 +2300,182 @@
         <v>12</v>
       </c>
       <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="46">
-        <v>1</v>
-      </c>
-      <c r="G27" s="46"/>
-      <c r="H27" s="10"/>
+      <c r="E27" s="32">
+        <v>13</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="46">
+        <v>1</v>
+      </c>
+      <c r="H27" s="46"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K27" s="10"/>
+      <c r="L27" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="C28">
         <v>8</v>
       </c>
-      <c r="F28" s="44">
-        <v>1</v>
-      </c>
-      <c r="K28" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E28" s="19">
+        <v>14</v>
+      </c>
+      <c r="G28" s="44">
+        <v>1</v>
+      </c>
+      <c r="L28" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>36</v>
       </c>
       <c r="C29">
         <v>7</v>
       </c>
-      <c r="K29" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E29" s="19">
+        <v>15</v>
+      </c>
+      <c r="L29" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>37</v>
       </c>
       <c r="C30">
         <v>9</v>
       </c>
-      <c r="K30" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E30" s="19">
+        <v>16</v>
+      </c>
+      <c r="L30" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>38</v>
       </c>
       <c r="C31">
         <v>7</v>
       </c>
-      <c r="F31" s="44">
-        <v>1</v>
-      </c>
-      <c r="K31" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E31" s="19">
+        <v>17</v>
+      </c>
+      <c r="G31" s="44">
+        <v>1</v>
+      </c>
+      <c r="L31" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>39</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="K32" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>40</v>
       </c>
       <c r="C33">
         <v>5</v>
       </c>
-      <c r="F33" s="44">
-        <v>1</v>
-      </c>
-      <c r="K33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>18</v>
+      </c>
+      <c r="G33" s="44">
+        <v>1</v>
+      </c>
+      <c r="L33" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>41</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>86</v>
       </c>
-      <c r="K34" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>42</v>
       </c>
       <c r="C35">
         <v>5</v>
       </c>
-      <c r="F35" s="44">
-        <v>1</v>
-      </c>
-      <c r="K35" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>19</v>
+      </c>
+      <c r="G35" s="44">
+        <v>1</v>
+      </c>
+      <c r="L35" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>43</v>
       </c>
       <c r="C36">
         <v>8</v>
       </c>
-      <c r="F36" s="44">
-        <v>1</v>
-      </c>
-      <c r="K36" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="G36" s="44">
+        <v>1</v>
+      </c>
+      <c r="L36" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>44</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
-      <c r="K37" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>78</v>
       </c>
@@ -2419,152 +2486,182 @@
         <v>6</v>
       </c>
       <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="46">
-        <v>1</v>
-      </c>
-      <c r="G38" s="46"/>
-      <c r="H38" s="10"/>
+      <c r="E38" s="32">
+        <v>21</v>
+      </c>
+      <c r="F38" s="32"/>
+      <c r="G38" s="46">
+        <v>1</v>
+      </c>
+      <c r="H38" s="46"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
-      <c r="K38" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K38" s="10"/>
+      <c r="L38" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>46</v>
       </c>
       <c r="C39">
         <v>6</v>
       </c>
-      <c r="F39" s="44">
-        <v>1</v>
-      </c>
-      <c r="K39" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E39" s="19">
+        <v>22</v>
+      </c>
+      <c r="G39" s="44">
+        <v>1</v>
+      </c>
+      <c r="L39" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>47</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
-      <c r="F40" s="44">
-        <v>1</v>
-      </c>
-      <c r="K40" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E40" s="19">
+        <v>23</v>
+      </c>
+      <c r="G40" s="44">
+        <v>1</v>
+      </c>
+      <c r="L40" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>48</v>
       </c>
       <c r="C41">
         <v>6</v>
       </c>
-      <c r="K41" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E41" s="19">
+        <v>24</v>
+      </c>
+      <c r="L41" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>49</v>
       </c>
       <c r="C42">
         <v>5</v>
       </c>
-      <c r="F42" s="44">
-        <v>1</v>
-      </c>
-      <c r="K42" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E42" s="19">
+        <v>25</v>
+      </c>
+      <c r="G42" s="44">
+        <v>1</v>
+      </c>
+      <c r="L42" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>50</v>
       </c>
       <c r="C43">
         <v>6</v>
       </c>
-      <c r="F43" s="44">
-        <v>1</v>
-      </c>
-      <c r="K43" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E43" s="19">
+        <v>26</v>
+      </c>
+      <c r="G43" s="44">
+        <v>1</v>
+      </c>
+      <c r="L43" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>51</v>
       </c>
       <c r="C44">
         <v>4</v>
       </c>
-      <c r="F44" s="44">
-        <v>1</v>
-      </c>
-      <c r="K44" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E44" s="19">
+        <v>27</v>
+      </c>
+      <c r="G44" s="44">
+        <v>1</v>
+      </c>
+      <c r="L44" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>52</v>
       </c>
       <c r="C45">
         <v>7</v>
       </c>
-      <c r="F45" s="44">
-        <v>1</v>
-      </c>
-      <c r="K45" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E45" s="19">
+        <v>28</v>
+      </c>
+      <c r="G45" s="44">
+        <v>1</v>
+      </c>
+      <c r="L45" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>53</v>
       </c>
       <c r="C46">
         <v>6</v>
       </c>
-      <c r="F46" s="44">
-        <v>1</v>
-      </c>
-      <c r="K46" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E46" s="19">
+        <v>29</v>
+      </c>
+      <c r="G46" s="44">
+        <v>1</v>
+      </c>
+      <c r="L46" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>54</v>
       </c>
       <c r="C47">
         <v>5</v>
       </c>
-      <c r="F47" s="44">
-        <v>1</v>
-      </c>
-      <c r="K47" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E47" s="19">
+        <v>30</v>
+      </c>
+      <c r="G47" s="44">
+        <v>1</v>
+      </c>
+      <c r="L47" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>77</v>
       </c>
@@ -2575,102 +2672,117 @@
         <v>2</v>
       </c>
       <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="46"/>
+      <c r="E48" s="32">
+        <v>31</v>
+      </c>
+      <c r="F48" s="32"/>
       <c r="G48" s="46"/>
-      <c r="H48" s="10"/>
+      <c r="H48" s="46"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
-      <c r="K48" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K48" s="10"/>
+      <c r="L48" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>56</v>
       </c>
       <c r="C49">
         <v>7</v>
       </c>
-      <c r="F49" s="44">
-        <v>1</v>
-      </c>
-      <c r="K49" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E49" s="19">
+        <v>32</v>
+      </c>
+      <c r="G49" s="44">
+        <v>1</v>
+      </c>
+      <c r="L49" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>57</v>
       </c>
       <c r="C50">
         <v>4</v>
       </c>
-      <c r="F50" s="44">
-        <v>1</v>
-      </c>
-      <c r="K50" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E50" s="19">
+        <v>33</v>
+      </c>
+      <c r="G50" s="44">
+        <v>1</v>
+      </c>
+      <c r="L50" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>58</v>
       </c>
       <c r="C51">
         <v>3</v>
       </c>
-      <c r="K51" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>59</v>
       </c>
       <c r="C52">
         <v>4</v>
       </c>
-      <c r="K52" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>60</v>
       </c>
       <c r="C53">
         <v>6</v>
       </c>
-      <c r="F53" s="44">
-        <v>1</v>
-      </c>
-      <c r="K53" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>34</v>
+      </c>
+      <c r="G53" s="44">
+        <v>1</v>
+      </c>
+      <c r="L53" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>61</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
-      <c r="F54" s="44">
-        <v>1</v>
-      </c>
-      <c r="K54" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>35</v>
+      </c>
+      <c r="G54" s="44">
+        <v>1</v>
+      </c>
+      <c r="L54" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
         <v>76</v>
       </c>
@@ -2681,62 +2793,71 @@
         <v>2</v>
       </c>
       <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="46">
-        <v>1</v>
-      </c>
-      <c r="G55" s="46"/>
-      <c r="H55" s="10"/>
+      <c r="E55" s="32">
+        <v>36</v>
+      </c>
+      <c r="F55" s="32"/>
+      <c r="G55" s="46">
+        <v>1</v>
+      </c>
+      <c r="H55" s="46"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
-      <c r="K55" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K55" s="10"/>
+      <c r="L55" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56">
         <v>7</v>
       </c>
-      <c r="F56" s="44">
-        <v>1</v>
-      </c>
-      <c r="K56" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E56" s="19">
+        <v>37</v>
+      </c>
+      <c r="G56" s="44">
+        <v>1</v>
+      </c>
+      <c r="L56" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>64</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
-      <c r="F57" s="44">
-        <v>1</v>
-      </c>
-      <c r="K57" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E57" s="19">
+        <v>38</v>
+      </c>
+      <c r="G57" s="44">
+        <v>1</v>
+      </c>
+      <c r="L57" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>65</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
-      <c r="K58" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
         <v>81</v>
       </c>
@@ -2747,33 +2868,39 @@
         <v>4</v>
       </c>
       <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="46"/>
+      <c r="E59" s="32">
+        <v>39</v>
+      </c>
+      <c r="F59" s="32"/>
       <c r="G59" s="46"/>
-      <c r="H59" s="10"/>
+      <c r="H59" s="46"/>
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K59" s="10"/>
+      <c r="L59" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>67</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
-      <c r="F60" s="44">
-        <v>1</v>
-      </c>
-      <c r="K60" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E60" s="19">
+        <v>40</v>
+      </c>
+      <c r="G60" s="44">
+        <v>1</v>
+      </c>
+      <c r="L60" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="31" t="s">
         <v>6</v>
       </c>
@@ -2785,37 +2912,38 @@
       </c>
       <c r="D61" s="32"/>
       <c r="E61" s="32"/>
-      <c r="F61" s="46">
-        <v>1</v>
-      </c>
-      <c r="G61" s="46"/>
-      <c r="H61" s="10"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="46">
+        <v>1</v>
+      </c>
+      <c r="H61" s="46"/>
       <c r="I61" s="10"/>
       <c r="J61" s="10"/>
-      <c r="K61" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K61" s="10"/>
+      <c r="L61" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>69</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>86</v>
       </c>
-      <c r="F62" s="44">
-        <v>1</v>
-      </c>
-      <c r="K62" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G62" s="44">
+        <v>1</v>
+      </c>
+      <c r="L62" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>70</v>
       </c>
@@ -2825,27 +2953,27 @@
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="F63" s="44">
-        <v>1</v>
-      </c>
-      <c r="K63" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G63" s="44">
+        <v>1</v>
+      </c>
+      <c r="L63" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>71</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
-      <c r="K64" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>72</v>
       </c>
@@ -2855,27 +2983,27 @@
       <c r="D65">
         <v>3</v>
       </c>
-      <c r="F65" s="44">
-        <v>1</v>
-      </c>
-      <c r="K65" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G65" s="44">
+        <v>1</v>
+      </c>
+      <c r="L65" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>73</v>
       </c>
       <c r="C66">
         <v>2</v>
       </c>
-      <c r="K66" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>74</v>
       </c>
@@ -2885,52 +3013,53 @@
       <c r="D67">
         <v>1</v>
       </c>
-      <c r="F67" s="44">
-        <v>1</v>
-      </c>
-      <c r="K67" s="35">
-        <f t="shared" ref="K67:K68" si="4">SUM(G67:J67)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G67" s="44">
+        <v>1</v>
+      </c>
+      <c r="L67" s="35">
+        <f t="shared" ref="L67:L68" si="4">SUM(H67:K67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>75</v>
       </c>
       <c r="C68">
         <v>3</v>
       </c>
-      <c r="F68" s="44">
-        <v>1</v>
-      </c>
-      <c r="K68" s="35">
+      <c r="G68" s="44">
+        <v>1</v>
+      </c>
+      <c r="L68" s="35">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="31"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
       <c r="E69" s="32"/>
-      <c r="F69" s="46"/>
+      <c r="F69" s="32"/>
       <c r="G69" s="46"/>
-      <c r="H69" s="10"/>
+      <c r="H69" s="46"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
-      <c r="K69" s="36"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="36"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:K100">
+  <conditionalFormatting sqref="B2:L100">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
-      <formula>$K2&gt;=(0.5+$N$21)</formula>
+      <formula>$L2&gt;=(0.5+$O$21)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>$K2&gt;=$N$21</formula>
+      <formula>$L2&gt;=$O$21</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$K2&gt;=($N$21-0.5)</formula>
+      <formula>$L2&gt;=($O$21-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweaked spreadsheet and notes.
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
@@ -220,9 +220,6 @@
     <t>11 Slowing Down, Speeding Up, and Turning . . . . . . . . . . . . . . . . . . . . . . . . . . . . . 52</t>
   </si>
   <si>
-    <t>12 Equations to De_x001C_ne Velocity and Acceleration . . . . . . . . . . . . . . . . . . . . . . . . . . 65</t>
-  </si>
-  <si>
     <t>13 Measurement and Uncertainty . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . 71</t>
   </si>
   <si>
@@ -438,10 +435,6 @@
 pages</t>
   </si>
   <si>
-    <t>Fall 2016
-TOTAL</t>
-  </si>
-  <si>
     <t>5 Determining Pi . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . . 15</t>
   </si>
   <si>
@@ -458,7 +451,16 @@
 Henry</t>
   </si>
   <si>
-    <t>number,
+    <t>12 Equations to Defi_x001C_ne Velocity and Acceleration . . . . . . . . . . . . . . . . . . . . . . . . . . 65</t>
+  </si>
+  <si>
+    <t>Fall 2016
+TOTAL
+USERS</t>
+  </si>
+  <si>
+    <t>Number
+in manual,
 fall 2015</t>
   </si>
 </sst>
@@ -1606,10 +1608,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="864" activePane="bottomLeft"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1152" activePane="bottomLeft"/>
+      <selection activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1619,8 @@
     <col min="1" max="1" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.5546875" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="8.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="44"/>
     <col min="8" max="8" width="8.21875" style="44" bestFit="1" customWidth="1"/>
@@ -1627,7 +1630,7 @@
     <col min="16" max="16" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
@@ -1635,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>99</v>
@@ -1647,22 +1650,22 @@
         <v>1</v>
       </c>
       <c r="G1" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="34" t="s">
         <v>98</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="N1" s="22" t="s">
         <v>4</v>
@@ -1680,10 +1683,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1718,7 +1721,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1760,7 +1763,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>12</v>
@@ -1886,7 +1889,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2073,7 +2076,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -2087,7 +2090,7 @@
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P15" s="5"/>
       <c r="Q15" s="9">
@@ -2096,7 +2099,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -2116,7 +2119,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -2133,7 +2136,7 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="43">
@@ -2142,7 +2145,7 @@
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P18" s="42"/>
       <c r="Q18" s="21">
@@ -2168,7 +2171,7 @@
     </row>
     <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -2181,7 +2184,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2197,7 +2200,7 @@
     </row>
     <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -2213,7 +2216,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2225,7 +2228,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -2237,7 +2240,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2255,13 +2258,13 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G25" s="44">
         <v>1</v>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -2291,10 +2294,10 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="32">
         <v>12</v>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -2336,7 +2339,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29">
         <v>7</v>
@@ -2351,7 +2354,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -2366,7 +2369,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31">
         <v>7</v>
@@ -2384,7 +2387,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -2396,7 +2399,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -2414,13 +2417,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L34" s="35">
         <f t="shared" si="0"/>
@@ -2429,7 +2432,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -2447,7 +2450,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36">
         <v>8</v>
@@ -2465,7 +2468,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -2477,10 +2480,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="32">
         <v>6</v>
@@ -2504,7 +2507,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -2522,7 +2525,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -2540,7 +2543,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -2555,7 +2558,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42">
         <v>5</v>
@@ -2573,7 +2576,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -2591,7 +2594,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44">
         <v>4</v>
@@ -2609,7 +2612,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45">
         <v>7</v>
@@ -2627,7 +2630,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -2645,7 +2648,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -2663,10 +2666,10 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="32">
         <v>2</v>
@@ -2688,7 +2691,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>7</v>
@@ -2706,7 +2709,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50">
         <v>4</v>
@@ -2724,7 +2727,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -2736,7 +2739,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -2748,7 +2751,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -2766,7 +2769,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -2784,10 +2787,10 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="32">
         <v>2</v>
@@ -2811,7 +2814,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56">
         <v>7</v>
@@ -2829,7 +2832,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -2847,7 +2850,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -2859,10 +2862,10 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="32">
         <v>4</v>
@@ -2884,7 +2887,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -2905,7 +2908,7 @@
         <v>6</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="32">
         <v>2</v>
@@ -2927,13 +2930,13 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G62" s="44">
         <v>1</v>
@@ -2945,7 +2948,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -2963,7 +2966,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2975,7 +2978,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65">
         <v>4</v>
@@ -2993,7 +2996,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -3005,7 +3008,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -3023,7 +3026,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68">
         <v>3</v>

</xml_diff>

<commit_message>
Added extra page breaks to title page
Title page and Table of Contents now appear on right hand pages.  Also
added current author addresses as footnote.  Updated page count in Excel
sheet accordingly.
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
@@ -1611,7 +1611,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1152" activePane="bottomLeft"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,7 +1689,7 @@
         <v>82</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="O3" s="6">
         <f>SUMIF(L$2:L$81,"&gt;=" &amp; N3,C$2:C$81)</f>
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="P3" s="6">
         <f>SUMIF(L$2:L$81,"&gt;=" &amp; N3,D$2:D$81)</f>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="Q3" s="9">
         <f>($Q$16 + $Q$14*O3+($Q$15)*P3)*(1+Q$17+Q$18)</f>
-        <v>25.350000000000005</v>
+        <v>25.480000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="O4" s="6">
         <f t="shared" ref="O4:O11" si="1">SUMIF(L$2:L$81,"&gt;=" &amp; N4,C$2:C$81)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P11" si="2">SUMIF(L$2:L$81,"&gt;=" &amp; N4,D$2:D$81)</f>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="Q4" s="9">
         <f t="shared" ref="Q4:Q11" si="3">($Q$16 + $Q$14*O4+($Q$15)*P4)*(1+Q$17+Q$18)</f>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1822,7 +1822,7 @@
       </c>
       <c r="O5" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="2"/>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="Q5" s="9">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="O6" s="19">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P6" s="19">
         <f t="shared" si="2"/>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="Q6" s="20">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="O7" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
@@ -1884,7 +1884,7 @@
       </c>
       <c r="Q7" s="9">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="O8" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="Q8" s="9">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="O9" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="Q9" s="9">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="O10" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="Q10" s="9">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="O11" s="11">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P11" s="11">
         <f t="shared" si="2"/>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="Q11" s="12">
         <f t="shared" si="3"/>
-        <v>4.55</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
spreadsheets for what labs to include 2016-17
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2016fall.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="131 lab list" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1275,7 +1276,28 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1609,9 +1631,9 @@
   <dimension ref="A1:R69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1152" activePane="bottomLeft"/>
+      <pane ySplit="1152" topLeftCell="A52" activePane="bottomLeft"/>
       <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1779,28 +1801,34 @@
       <c r="G4" s="46">
         <v>1</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="10"/>
+      <c r="H4" s="46">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="K4" s="10">
+        <v>0.5</v>
+      </c>
       <c r="L4" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="N4" s="23">
         <v>0.5</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" ref="O4:O11" si="1">SUMIF(L$2:L$81,"&gt;=" &amp; N4,C$2:C$81)</f>
-        <v>6</v>
+        <v>270</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ref="P4:P11" si="2">SUMIF(L$2:L$81,"&gt;=" &amp; N4,D$2:D$81)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q4" s="9">
         <f t="shared" ref="Q4:Q11" si="3">($Q$16 + $Q$14*O4+($Q$15)*P4)*(1+Q$17+Q$18)</f>
-        <v>4.68</v>
+        <v>23.790000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1813,24 +1841,27 @@
       <c r="E5">
         <v>2</v>
       </c>
+      <c r="K5" s="2">
+        <v>0.75</v>
+      </c>
       <c r="L5" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N5" s="23">
         <v>1</v>
       </c>
       <c r="O5" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="9">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>22.230000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1840,6 +1871,9 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
       <c r="L6" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1849,15 +1883,15 @@
       </c>
       <c r="O6" s="19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>214</v>
       </c>
       <c r="P6" s="19">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="20">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>20.150000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1867,6 +1901,9 @@
       <c r="C7">
         <v>2</v>
       </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
       <c r="L7" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1876,15 +1913,15 @@
       </c>
       <c r="O7" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q7" s="9">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>18.134999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1894,6 +1931,9 @@
       <c r="C8">
         <v>2</v>
       </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
       <c r="L8" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1903,15 +1943,15 @@
       </c>
       <c r="O8" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="9">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>17.094999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1927,24 +1967,36 @@
       <c r="G9" s="44">
         <v>1</v>
       </c>
+      <c r="H9" s="44">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
       <c r="L9" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N9" s="23">
         <v>3</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="9">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>15.340000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1960,24 +2012,36 @@
       <c r="G10" s="44">
         <v>1</v>
       </c>
+      <c r="H10" s="44">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
       <c r="L10" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N10" s="23">
         <v>3.5</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q10" s="9">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>12.480000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1993,24 +2057,33 @@
       <c r="G11" s="44">
         <v>1</v>
       </c>
+      <c r="H11" s="44">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.75</v>
+      </c>
       <c r="L11" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="N11" s="25">
         <v>4</v>
       </c>
       <c r="O11" s="11">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="P11" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q11" s="12">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -2020,9 +2093,15 @@
       <c r="C12">
         <v>3</v>
       </c>
+      <c r="J12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
       <c r="L12" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N12" s="3"/>
     </row>
@@ -2039,9 +2118,18 @@
       <c r="G13" s="44">
         <v>1</v>
       </c>
+      <c r="H13" s="44">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
       <c r="L13" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="1" t="s">
@@ -2061,9 +2149,18 @@
       <c r="G14" s="44">
         <v>1</v>
       </c>
+      <c r="H14" s="44">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L14" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="14" t="s">
@@ -2084,6 +2181,9 @@
       <c r="E15">
         <v>8</v>
       </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
       <c r="L15" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2104,9 +2204,15 @@
       <c r="C16">
         <v>3</v>
       </c>
+      <c r="J16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
       <c r="L16" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="15" t="s">
@@ -2130,9 +2236,15 @@
       <c r="G17" s="44">
         <v>1</v>
       </c>
+      <c r="H17" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.75</v>
+      </c>
       <c r="L17" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="15" t="s">
@@ -2156,9 +2268,21 @@
       <c r="G18" s="44">
         <v>1</v>
       </c>
+      <c r="H18" s="44">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.75</v>
+      </c>
       <c r="L18" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="16" t="s">
@@ -2176,6 +2300,9 @@
       <c r="C19">
         <v>2</v>
       </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
       <c r="L19" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2189,6 +2316,9 @@
       <c r="C20">
         <v>1</v>
       </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
       <c r="L20" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2205,6 +2335,9 @@
       <c r="C21">
         <v>2</v>
       </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
       <c r="L21" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2221,9 +2354,15 @@
       <c r="C22">
         <v>1</v>
       </c>
+      <c r="J22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
       <c r="L22" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -2233,6 +2372,9 @@
       <c r="C23">
         <v>2</v>
       </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
       <c r="L23" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2251,9 +2393,21 @@
       <c r="G24" s="44">
         <v>1</v>
       </c>
+      <c r="H24" s="44">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
       <c r="L24" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -2269,9 +2423,15 @@
       <c r="G25" s="44">
         <v>1</v>
       </c>
+      <c r="H25" s="44">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
       <c r="L25" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -2287,9 +2447,18 @@
       <c r="G26" s="44">
         <v>1</v>
       </c>
+      <c r="H26" s="44">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
       <c r="L26" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2310,13 +2479,21 @@
       <c r="G27" s="46">
         <v>1</v>
       </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="H27" s="46">
+        <v>1</v>
+      </c>
+      <c r="I27" s="10">
+        <v>1</v>
+      </c>
+      <c r="J27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="10">
+        <v>1</v>
+      </c>
       <c r="L27" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2332,9 +2509,15 @@
       <c r="G28" s="44">
         <v>1</v>
       </c>
+      <c r="H28" s="44">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.8</v>
+      </c>
       <c r="L28" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2347,9 +2530,12 @@
       <c r="E29" s="19">
         <v>15</v>
       </c>
+      <c r="K29" s="2">
+        <v>0.7</v>
+      </c>
       <c r="L29" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2362,9 +2548,15 @@
       <c r="E30" s="19">
         <v>16</v>
       </c>
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L30" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2380,9 +2572,21 @@
       <c r="G31" s="44">
         <v>1</v>
       </c>
+      <c r="H31" s="44">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L31" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2392,9 +2596,12 @@
       <c r="C32">
         <v>4</v>
       </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
       <c r="L32" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -2410,9 +2617,21 @@
       <c r="G33" s="44">
         <v>1</v>
       </c>
+      <c r="H33" s="44">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L33" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2425,9 +2644,15 @@
       <c r="F34" t="s">
         <v>85</v>
       </c>
+      <c r="I34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L34" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2443,9 +2668,18 @@
       <c r="G35" s="44">
         <v>1</v>
       </c>
+      <c r="H35" s="44">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1</v>
+      </c>
       <c r="L35" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -2461,9 +2695,15 @@
       <c r="G36" s="44">
         <v>1</v>
       </c>
+      <c r="H36" s="44">
+        <v>1</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L36" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -2473,9 +2713,18 @@
       <c r="C37">
         <v>4</v>
       </c>
+      <c r="I37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0.8</v>
+      </c>
       <c r="L37" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -2496,13 +2745,21 @@
       <c r="G38" s="46">
         <v>1</v>
       </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
+      <c r="H38" s="46">
+        <v>1</v>
+      </c>
+      <c r="I38" s="10">
+        <v>1</v>
+      </c>
+      <c r="J38" s="10">
+        <v>1</v>
+      </c>
+      <c r="K38" s="10">
+        <v>1</v>
+      </c>
       <c r="L38" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2518,9 +2775,18 @@
       <c r="G39" s="44">
         <v>1</v>
       </c>
+      <c r="H39" s="44">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0.75</v>
+      </c>
       <c r="L39" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -2536,9 +2802,21 @@
       <c r="G40" s="44">
         <v>1</v>
       </c>
+      <c r="H40" s="44">
+        <v>1</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K40" s="2">
+        <v>0.5</v>
+      </c>
       <c r="L40" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -2551,9 +2829,12 @@
       <c r="E41" s="19">
         <v>24</v>
       </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
       <c r="L41" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -2569,9 +2850,21 @@
       <c r="G42" s="44">
         <v>1</v>
       </c>
+      <c r="H42" s="44">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>1</v>
+      </c>
+      <c r="J42" s="2">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
       <c r="L42" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -2587,9 +2880,18 @@
       <c r="G43" s="44">
         <v>1</v>
       </c>
+      <c r="H43" s="44">
+        <v>1</v>
+      </c>
+      <c r="J43" s="2">
+        <v>1</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1</v>
+      </c>
       <c r="L43" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -2605,9 +2907,18 @@
       <c r="G44" s="44">
         <v>1</v>
       </c>
+      <c r="H44" s="44">
+        <v>1</v>
+      </c>
+      <c r="J44" s="2">
+        <v>1</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0.75</v>
+      </c>
       <c r="L44" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -2623,9 +2934,21 @@
       <c r="G45" s="44">
         <v>1</v>
       </c>
+      <c r="H45" s="44">
+        <v>1</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2">
+        <v>1</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1</v>
+      </c>
       <c r="L45" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -2641,9 +2964,18 @@
       <c r="G46" s="44">
         <v>1</v>
       </c>
+      <c r="I46" s="2">
+        <v>1</v>
+      </c>
+      <c r="J46" s="2">
+        <v>1</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0</v>
+      </c>
       <c r="L46" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -2659,9 +2991,21 @@
       <c r="G47" s="44">
         <v>1</v>
       </c>
+      <c r="H47" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
       <c r="L47" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -2681,12 +3025,18 @@
       <c r="F48" s="32"/>
       <c r="G48" s="46"/>
       <c r="H48" s="46"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
+      <c r="I48" s="10">
+        <v>1</v>
+      </c>
+      <c r="J48" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K48" s="10">
+        <v>0</v>
+      </c>
       <c r="L48" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2702,9 +3052,21 @@
       <c r="G49" s="44">
         <v>1</v>
       </c>
+      <c r="H49" s="44">
+        <v>1</v>
+      </c>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="2">
+        <v>1</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0.7</v>
+      </c>
       <c r="L49" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -2720,9 +3082,21 @@
       <c r="G50" s="44">
         <v>1</v>
       </c>
+      <c r="H50" s="44">
+        <v>1</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2">
+        <v>1</v>
+      </c>
+      <c r="K50" s="2">
+        <v>1</v>
+      </c>
       <c r="L50" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -2732,9 +3106,15 @@
       <c r="C51">
         <v>3</v>
       </c>
+      <c r="J51" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="2">
+        <v>0</v>
+      </c>
       <c r="L51" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -2744,6 +3124,9 @@
       <c r="C52">
         <v>4</v>
       </c>
+      <c r="K52" s="2">
+        <v>0</v>
+      </c>
       <c r="L52" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2762,9 +3145,12 @@
       <c r="G53" s="44">
         <v>1</v>
       </c>
+      <c r="K53" s="2">
+        <v>0.7</v>
+      </c>
       <c r="L53" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -2780,9 +3166,21 @@
       <c r="G54" s="44">
         <v>1</v>
       </c>
+      <c r="H54" s="44">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2">
+        <v>1</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1</v>
+      </c>
+      <c r="K54" s="2">
+        <v>1</v>
+      </c>
       <c r="L54" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -2805,11 +3203,15 @@
       </c>
       <c r="H55" s="46"/>
       <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
+      <c r="J55" s="10">
+        <v>1</v>
+      </c>
+      <c r="K55" s="10">
+        <v>1</v>
+      </c>
       <c r="L55" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -2825,9 +3227,21 @@
       <c r="G56" s="44">
         <v>1</v>
       </c>
+      <c r="H56" s="44">
+        <v>1</v>
+      </c>
+      <c r="I56" s="2">
+        <v>1</v>
+      </c>
+      <c r="J56" s="2">
+        <v>1</v>
+      </c>
+      <c r="K56" s="2">
+        <v>1</v>
+      </c>
       <c r="L56" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -2843,9 +3257,21 @@
       <c r="G57" s="44">
         <v>1</v>
       </c>
+      <c r="H57" s="44">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2">
+        <v>1</v>
+      </c>
+      <c r="J57" s="2">
+        <v>1</v>
+      </c>
+      <c r="K57" s="2">
+        <v>1</v>
+      </c>
       <c r="L57" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -2855,6 +3281,9 @@
       <c r="C58">
         <v>3</v>
       </c>
+      <c r="K58" s="2">
+        <v>0</v>
+      </c>
       <c r="L58" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2877,12 +3306,16 @@
       <c r="F59" s="32"/>
       <c r="G59" s="46"/>
       <c r="H59" s="46"/>
-      <c r="I59" s="10"/>
+      <c r="I59" s="10">
+        <v>1</v>
+      </c>
       <c r="J59" s="10"/>
-      <c r="K59" s="10"/>
+      <c r="K59" s="10">
+        <v>0</v>
+      </c>
       <c r="L59" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -2898,9 +3331,15 @@
       <c r="G60" s="44">
         <v>1</v>
       </c>
+      <c r="I60" s="2">
+        <v>1</v>
+      </c>
+      <c r="K60" s="2">
+        <v>0</v>
+      </c>
       <c r="L60" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -2919,13 +3358,19 @@
       <c r="G61" s="46">
         <v>1</v>
       </c>
-      <c r="H61" s="46"/>
+      <c r="H61" s="46">
+        <v>1</v>
+      </c>
       <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
+      <c r="J61" s="10">
+        <v>1</v>
+      </c>
+      <c r="K61" s="10">
+        <v>1</v>
+      </c>
       <c r="L61" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -2941,9 +3386,15 @@
       <c r="G62" s="44">
         <v>1</v>
       </c>
+      <c r="J62" s="2">
+        <v>1</v>
+      </c>
+      <c r="K62" s="2">
+        <v>0</v>
+      </c>
       <c r="L62" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -2959,9 +3410,21 @@
       <c r="G63" s="44">
         <v>1</v>
       </c>
+      <c r="H63" s="44">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2">
+        <v>1</v>
+      </c>
       <c r="L63" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -2971,9 +3434,12 @@
       <c r="C64">
         <v>1</v>
       </c>
+      <c r="K64" s="2">
+        <v>1</v>
+      </c>
       <c r="L64" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -2989,9 +3455,21 @@
       <c r="G65" s="44">
         <v>1</v>
       </c>
+      <c r="H65" s="44">
+        <v>1</v>
+      </c>
+      <c r="I65" s="2">
+        <v>1</v>
+      </c>
+      <c r="J65" s="2">
+        <v>1</v>
+      </c>
+      <c r="K65" s="2">
+        <v>1</v>
+      </c>
       <c r="L65" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -3001,9 +3479,12 @@
       <c r="C66">
         <v>2</v>
       </c>
+      <c r="K66" s="2">
+        <v>1</v>
+      </c>
       <c r="L66" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -3019,9 +3500,21 @@
       <c r="G67" s="44">
         <v>1</v>
       </c>
+      <c r="H67" s="44">
+        <v>1</v>
+      </c>
+      <c r="I67" s="2">
+        <v>1</v>
+      </c>
+      <c r="J67" s="2">
+        <v>1</v>
+      </c>
+      <c r="K67" s="2">
+        <v>1</v>
+      </c>
       <c r="L67" s="35">
         <f t="shared" ref="L67:L68" si="4">SUM(H67:K67)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -3034,9 +3527,21 @@
       <c r="G68" s="44">
         <v>1</v>
       </c>
+      <c r="H68" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="I68" s="2">
+        <v>1</v>
+      </c>
+      <c r="J68" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K68" s="2">
+        <v>0</v>
+      </c>
       <c r="L68" s="35">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -3055,17 +3560,456 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:L100">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>$L2&gt;=(0.5+$O$21)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>$L2&gt;=$O$21</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$L2&gt;=($O$21-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G2:I68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:I68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <v>0.5</v>
+      </c>
+      <c r="I37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G47">
+        <v>0.5</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I51">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="54" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>0.5</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>